<commit_message>
Create map of ship. Ignore enter.
</commit_message>
<xml_diff>
--- a/day25/ship.xlsx
+++ b/day25/ship.xlsx
@@ -16,26 +16,74 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>start</t>
   </si>
   <si>
-    <t>wrapping</t>
-  </si>
-  <si>
-    <t>corridor</t>
-  </si>
-  <si>
-    <t>lab</t>
+    <t>molten lava</t>
+  </si>
+  <si>
+    <t>mutex</t>
+  </si>
+  <si>
+    <t>infinite loop</t>
+  </si>
+  <si>
+    <t>astrolabe</t>
+  </si>
+  <si>
+    <t>dehydrated water</t>
+  </si>
+  <si>
+    <t>escape pod</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>wreath</t>
+  </si>
+  <si>
+    <t>monolith</t>
+  </si>
+  <si>
+    <t>asterisk</t>
+  </si>
+  <si>
+    <t>photons</t>
+  </si>
+  <si>
+    <t>coin</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>? Leads to "astronaut ice cream" and security check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -51,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -60,12 +108,86 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color auto="1"/>
+      </left>
+      <right style="mediumDashed">
+        <color auto="1"/>
+      </right>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thick">
         <color auto="1"/>
       </left>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -74,12 +196,18 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top style="thick">
         <color auto="1"/>
       </top>
@@ -87,38 +215,63 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="mediumDashed">
         <color auto="1"/>
       </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,34 +574,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="K16:L19"/>
+  <dimension ref="B4:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="10.88671875" style="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="11:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K17" s="4" t="s">
+    <row r="4" spans="2:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:9" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="11:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="K18" s="2" t="s">
+    <row r="6" spans="2:9" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>1</v>
       </c>
+      <c r="I6" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="19" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="K19" s="3" t="s">
+    <row r="7" spans="2:9" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>0</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="6"/>
+      <c r="H8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solve day25 part 1 (and 2).
</commit_message>
<xml_diff>
--- a/day25/ship.xlsx
+++ b/day25/ship.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>start</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>? Leads to "astronaut ice cream" and security check</t>
+  </si>
+  <si>
+    <t>monolith + astronaut ice cream &lt; x</t>
+  </si>
+  <si>
+    <t>monolith + astronaut ice cream + wreath &gt; x</t>
+  </si>
+  <si>
+    <t>monolith + wreath &lt; x</t>
+  </si>
+  <si>
+    <t>astronaut ice cream + wreath &lt; x</t>
   </si>
 </sst>
 </file>
@@ -229,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -272,6 +284,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,21 +589,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:I11"/>
+  <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" style="1"/>
     <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.88671875" style="1"/>
+    <col min="3" max="10" width="10.88671875" style="1"/>
+    <col min="11" max="11" width="93.88671875" style="15" customWidth="1"/>
+    <col min="12" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:9" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K4" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E5" s="10" t="s">
         <v>8</v>
       </c>
@@ -605,7 +641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F6" s="7" t="s">
         <v>6</v>
       </c>
@@ -619,7 +655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="G7" s="14" t="s">
         <v>12</v>
       </c>
@@ -630,7 +666,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G8" s="6"/>
       <c r="H8" s="11" t="s">
         <v>9</v>
@@ -639,8 +675,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>